<commit_message>
fixed GET STARTED link
</commit_message>
<xml_diff>
--- a/public/background_slideshow/background_image_data.xlsx
+++ b/public/background_slideshow/background_image_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15413\Desktop\psu_shpe_website-main\psu_shpe_website-main\public\background_slideshow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F52D5D3-3EFF-456A-A0FD-478318F242A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AD5AF0-D634-4859-A75E-9F9C0A4B69B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="4150" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="62205" yWindow="8835" windowWidth="28800" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,9 +49,6 @@
     <t>external</t>
   </si>
   <si>
-    <t>https://www.pdx.edu/civil-environmental-engineering/student-orgs</t>
-  </si>
-  <si>
     <t>DISCOVER OUR COMMUNITY</t>
   </si>
   <si>
@@ -113,6 +110,9 @@
   </si>
   <si>
     <t>PORTLAND STATE UNIVERSITY</t>
+  </si>
+  <si>
+    <t>https://www.pdx.edu/</t>
   </si>
 </sst>
 </file>
@@ -422,7 +422,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -447,24 +447,24 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
@@ -475,88 +475,88 @@
       <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
+      <c r="E2" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="7" t="s">
-        <v>29</v>
-      </c>
       <c r="K2" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="7" t="s">
-        <v>29</v>
-      </c>
       <c r="K3" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="7" t="s">
-        <v>29</v>
-      </c>
       <c r="K4" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>